<commit_message>
Correct electric motor capital cost factor in indst/IECCpUAEU (#322)
</commit_message>
<xml_diff>
--- a/InputData/indst/IECCpUAEU/Indst Eqpt Cap Cost per Unit Ann E Use.xlsx
+++ b/InputData/indst/IECCpUAEU/Indst Eqpt Cap Cost per Unit Ann E Use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffRissman\CodeRepositories\eps-us\InputData\indst\IECCpUAEU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffRissman\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC49DAD-8EC2-4972-8D6D-74C169019BFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913FADC-8114-409A-98A0-C5A4C9DE821B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="345" windowWidth="37395" windowHeight="22410" xr2:uid="{6A73F6BA-E2AF-4EFC-B7D0-AD586970A910}"/>
+    <workbookView xWindow="10440" yWindow="1410" windowWidth="40695" windowHeight="21765" xr2:uid="{6A73F6BA-E2AF-4EFC-B7D0-AD586970A910}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -62,10 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="391">
-  <si>
-    <t>IECCpUAEU Industrial Equipment Capital Cost per Unit Annual Energy Use</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="401">
   <si>
     <t>Sources:</t>
   </si>
@@ -532,15 +529,6 @@
     <t>equiv. HP</t>
   </si>
   <si>
-    <t>Weighted Average for electric motors/drive units:</t>
-  </si>
-  <si>
-    <t>HP bins represented are 1-5, 6-20, 21-50,101-200,1000+. Not represented are 51-100 (2.9% of motor stock), 201-500 (0.7%), 501-1000 (0.2%). Weighted averages thus take % of motor inventory in a given HP bin and divide by 96.2%; weighted averages also average the values within a bin.</t>
-  </si>
-  <si>
-    <t>Operating hours, and percentage of motors in a given horsepower bin for calculating weighted averages,</t>
-  </si>
-  <si>
     <t>The recent assessment did not have data disaggregated in the appropriate way to provide more recent values.</t>
   </si>
   <si>
@@ -1216,9 +1204,6 @@
     <t>Adjustment to Operating Hours per Year</t>
   </si>
   <si>
-    <t>It seems reasonable that machine drive (light green) is more expensive than other end uses, given that it's producing rotational kinetic energy rather than heat or cooling.</t>
-  </si>
-  <si>
     <t>fully commercialized, electrified, high-temperature heating equipment.  For instance, cement kilns burn coal and steam crackers use natural gas.  Other electrical furnaces</t>
   </si>
   <si>
@@ -1226,9 +1211,6 @@
   </si>
   <si>
     <t>exist (like induction furnaces), but electric arc furnaces are likely the most common type and are likely the best choice to use as our model equipment type for high-temp</t>
-  </si>
-  <si>
-    <t>electrified industrial heating equipment. So we do not consider them to bean outlier - i.e., the higher cost is justified.</t>
   </si>
   <si>
     <t>Note: since the CapEx here scales with tonnes capacity, the final cost per unit capacity isn't affected by the annual production capacity figure above.</t>
@@ -1258,6 +1240,54 @@
       <t xml:space="preserve"> because it is the whole plant, not just the kiln.  Kiln-only data are just below.</t>
     </r>
   </si>
+  <si>
+    <t>Annual energy delivered (MMbtu)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% Distr. by Energy Use of Motor HP Category </t>
+  </si>
+  <si>
+    <t>Operating hours, and percentage of motors in a given horsepower bin for calculating weighted averages based on energy distribution,</t>
+  </si>
+  <si>
+    <t>Representative Horsepower Bin</t>
+  </si>
+  <si>
+    <t>101-200</t>
+  </si>
+  <si>
+    <t>21-50</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>6-20</t>
+  </si>
+  <si>
+    <t>1000+</t>
+  </si>
+  <si>
+    <t>$/BTU/yr</t>
+  </si>
+  <si>
+    <t>Weighted Average (by distribution of energy use) for electric motors/drive units (see below for breakdown):</t>
+  </si>
+  <si>
+    <t>Bins represented in the data by horsepower (HP) are 1-5, 6-20, 21-50,101-200,1000+. Not represented are 51-100 (12.7% of motor energy use), 201-500 (15.8%), 501-1000 (13.4%). Weighted averages thus take % of motor energy use in a given HP bin and divide by the remaining 58.1%. Weighted averages also average the energy values within a bin (e.g., averaging $/BTU/yr across all equipment in the 101-200 HP bin).</t>
+  </si>
+  <si>
+    <t>% Distr. by Energy Use Per HP Bin</t>
+  </si>
+  <si>
+    <t>Average Annual Energy Delivered by HP Bin (MMbtu)</t>
+  </si>
+  <si>
+    <t>electrified industrial heating equipment. So we do not consider them to be an outlier - i.e., the higher cost is justified.</t>
+  </si>
+  <si>
+    <t>IECCpUAEU Industrial Equipment Capital Cost per Unit Annual Energy Use</t>
+  </si>
 </sst>
 </file>
 
@@ -1269,7 +1299,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1331,8 +1361,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1393,8 +1438,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1426,13 +1476,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1504,16 +1607,44 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="3" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="11" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="8" fillId="11" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="11" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="8" fillId="11" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="11" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="11" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="11" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="11" borderId="6" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -2209,7 +2340,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.4733459973606227E-4</c:v>
+                  <c:v>2.9652197760109964E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7.0734511678239686E-5</c:v>
@@ -3271,23 +3402,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>185146</xdr:colOff>
       <xdr:row>130</xdr:row>
-      <xdr:rowOff>120400</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{950AD3EF-C451-057E-3713-FD08E757AEE3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C91347AF-CFB1-2100-496E-C236D3AEE0E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3310,8 +3441,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="647700" y="22075140"/>
-          <a:ext cx="7991475" cy="2429260"/>
+          <a:off x="548640" y="22539960"/>
+          <a:ext cx="7927066" cy="2423160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3716,20 +3847,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3739,22 +3870,22 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3764,27 +3895,27 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -3794,27 +3925,27 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
@@ -3824,27 +3955,27 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
@@ -3854,67 +3985,67 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -3924,22 +4055,22 @@
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="15" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
@@ -3949,32 +4080,32 @@
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="15" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
@@ -3984,12 +4115,12 @@
     </row>
     <row r="64" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="35" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
@@ -3997,12 +4128,12 @@
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
@@ -4012,17 +4143,17 @@
     </row>
     <row r="70" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="35" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
@@ -4030,12 +4161,12 @@
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
@@ -4045,12 +4176,12 @@
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="36" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B78" s="37" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
@@ -4058,12 +4189,12 @@
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
@@ -4073,7 +4204,7 @@
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
@@ -4081,7 +4212,7 @@
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
@@ -4091,22 +4222,22 @@
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
@@ -4116,27 +4247,27 @@
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="36" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
@@ -4146,12 +4277,12 @@
     </row>
     <row r="101" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B101" s="36" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="102" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B102" s="37" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
@@ -4159,32 +4290,32 @@
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="16" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
@@ -4194,47 +4325,47 @@
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>158</v>
+        <v>387</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="15" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="15" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -4281,7 +4412,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -4289,12 +4420,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4302,18 +4433,18 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>56603</v>
@@ -4328,7 +4459,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>25717</v>
@@ -4343,7 +4474,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>60507</v>
@@ -4358,7 +4489,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <f>AVERAGE(B6:B8)</f>
@@ -4375,17 +4506,17 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4393,15 +4524,15 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -4410,12 +4541,12 @@
         <v>5.6711966224873446E-5</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="18"/>
@@ -4424,12 +4555,12 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B24" s="8">
         <v>80375</v>
@@ -4437,7 +4568,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B25" s="8">
         <v>91475</v>
@@ -4445,7 +4576,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B26" s="8">
         <f>AVERAGE(B24:B25)</f>
@@ -4454,7 +4585,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B28">
         <v>400</v>
@@ -4462,7 +4593,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B29">
         <v>0.74570000000000003</v>
@@ -4470,7 +4601,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B30">
         <f>B28*B29</f>
@@ -4479,7 +4610,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="22">
         <v>5280</v>
@@ -4487,42 +4618,42 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B34">
         <f>B30*B32</f>
         <v>1574918.4000000001</v>
       </c>
       <c r="C34" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35">
         <v>3412.14</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B36">
         <f>B34*B35</f>
         <v>5373842069.3760004</v>
       </c>
       <c r="C36" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -4531,12 +4662,12 @@
         <v>1.5989491110961776E-5</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18"/>
@@ -4545,27 +4676,27 @@
     </row>
     <row r="42" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="F42" s="23" t="s">
-        <v>70</v>
-      </c>
       <c r="G42" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43">
         <v>2000</v>
@@ -4591,7 +4722,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44">
         <v>2000</v>
@@ -4617,7 +4748,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B45">
         <v>2000</v>
@@ -4643,60 +4774,60 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B48">
         <f>B43*B32</f>
         <v>10560000</v>
       </c>
       <c r="C48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B49">
         <v>3412.14</v>
       </c>
       <c r="C49" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B50">
         <f>B48*B49</f>
         <v>36032198400</v>
       </c>
       <c r="C50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B55" s="18"/>
       <c r="C55" s="18"/>
@@ -4704,13 +4835,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" s="20"/>
     </row>
@@ -4720,7 +4851,7 @@
         <v>2.3984236666442662E-5</v>
       </c>
       <c r="B60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -4742,330 +4873,330 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="8">
         <v>307500</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>4000</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="8">
         <v>75863</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="8">
         <v>6226</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B11" s="25">
         <v>0.45</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B12" s="25">
         <v>0.15</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="21">
         <f>B8/B11</f>
         <v>168584.44444444444</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="21">
         <f>B9/B12</f>
         <v>41506.666666666672</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17">
         <v>100000</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18">
         <v>3412.14</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="9">
         <f>B14*B17</f>
         <v>16858444444.444445</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" s="9">
         <f>B15*B18</f>
         <v>141626557.60000002</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B26" s="9">
         <f>SUM(B20:B21)</f>
         <v>17000071002.044445</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="12">
         <f>B5/B26</f>
         <v>1.8088159747275158E-5</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B32" s="8">
         <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="8">
         <v>500</v>
       </c>
       <c r="C33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="8">
         <f>AVERAGE(B32:B33)</f>
         <v>350</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36">
         <v>500</v>
       </c>
       <c r="C36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B38" s="8">
         <f>B34*B36</f>
         <v>175000</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B41">
         <v>0.57599999999999996</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42">
         <f>B41*B36</f>
         <v>288</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44">
         <f>B6</f>
         <v>4000</v>
       </c>
       <c r="C44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B46">
         <f>B42*B44</f>
         <v>1152000</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B47" s="9">
         <f>B46*B18</f>
         <v>3930785280</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="12">
         <f>B38/B47</f>
         <v>4.4520366169683022E-5</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -5092,131 +5223,131 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>347</v>
-      </c>
-      <c r="B3" s="43"/>
+      <c r="A3" s="41" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="42"/>
       <c r="C3" s="11" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B5">
         <v>492000</v>
       </c>
-      <c r="C5" s="44"/>
+      <c r="C5" s="43"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B6">
         <v>135000</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="43"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B7">
         <v>474000</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="43"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B8">
         <v>70000</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B9">
         <v>22000</v>
       </c>
-      <c r="C9" s="44"/>
+      <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B10">
         <v>18000</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="43"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B11">
         <v>216000</v>
       </c>
-      <c r="C11" s="44"/>
+      <c r="C11" s="43"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B12">
         <v>51000</v>
       </c>
-      <c r="C12" s="44"/>
+      <c r="C12" s="43"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B13">
         <v>125000</v>
       </c>
-      <c r="C13" s="44"/>
+      <c r="C13" s="43"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
-        <v>361</v>
-      </c>
-      <c r="B15" s="43"/>
+      <c r="A15" s="41" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" s="42"/>
       <c r="C15" s="11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B17" s="20">
         <v>13400</v>
@@ -5224,7 +5355,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B18" s="20">
         <v>5300</v>
@@ -5232,40 +5363,40 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B19" s="20">
         <v>13600</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="41" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="11" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B23">
         <v>4380</v>
@@ -5276,7 +5407,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B24">
         <v>4380</v>
@@ -5287,7 +5418,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -5295,32 +5426,32 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B33" s="1">
         <f>Boilers!B32</f>
@@ -5329,43 +5460,43 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="47">
+        <v>54</v>
+      </c>
+      <c r="B36" s="46">
         <v>3412.14</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="32"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="46" t="s">
-        <v>371</v>
-      </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
+      <c r="A38" s="45" t="s">
+        <v>367</v>
+      </c>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B40">
         <f>$B$33*D23*B36</f>
@@ -5382,7 +5513,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B41">
         <f>$B$33*C24</f>
@@ -5399,50 +5530,50 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="42" t="s">
-        <v>357</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
+      <c r="A51" s="41" t="s">
+        <v>353</v>
+      </c>
+      <c r="B51" s="42"/>
+      <c r="C51" s="42"/>
       <c r="D51" s="11" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B53">
         <v>722000</v>
       </c>
-      <c r="C53" s="44">
+      <c r="C53" s="43">
         <f>B53/SUM($B$53:$B$54)</f>
         <v>0.45012468827930174</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B54">
         <v>882000</v>
       </c>
-      <c r="C54" s="44">
+      <c r="C54" s="43">
         <f>B54/SUM($B$53:$B$54)</f>
         <v>0.54987531172069826</v>
       </c>
@@ -5468,7 +5599,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -5479,12 +5610,12 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I2" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C3" s="25"/>
       <c r="F3" s="25">
@@ -5492,107 +5623,107 @@
         <v>264.16000000000003</v>
       </c>
       <c r="G3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F4">
         <v>450</v>
       </c>
       <c r="G4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C5" s="32"/>
       <c r="F5" s="32">
         <v>800000</v>
       </c>
       <c r="G5" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F7">
         <f>F4*F5</f>
         <v>360000000</v>
       </c>
       <c r="G7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F8">
         <f>F7*0.003412</f>
         <v>1228320</v>
       </c>
       <c r="G8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F9" s="25">
         <f>F3*F5</f>
         <v>211328000.00000003</v>
       </c>
       <c r="G9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F10" s="12">
         <f>F9/(F8*10^6)</f>
         <v>1.7204637228083889E-4</v>
       </c>
       <c r="G10" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E12">
         <f>8760*155</f>
         <v>1357800</v>
       </c>
       <c r="F12" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -5603,13 +5734,13 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F16" s="20">
         <v>170</v>
       </c>
       <c r="G16" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -5618,7 +5749,7 @@
         <v>26.356589147286826</v>
       </c>
       <c r="G17" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -5627,7 +5758,7 @@
         <v>9.4883645023316546E-2</v>
       </c>
       <c r="G18" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -5636,80 +5767,80 @@
         <v>2.7808805692648461E-5</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F21">
         <v>36000000</v>
       </c>
       <c r="G21" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F22" s="20">
         <f>F21*0.14</f>
         <v>5040000.0000000009</v>
       </c>
       <c r="G22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F23">
         <f>AVERAGE(5.1,7.8)</f>
         <v>6.4499999999999993</v>
       </c>
       <c r="G23" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I23" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F24">
         <v>8000</v>
       </c>
       <c r="G24" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F25">
         <v>600</v>
       </c>
       <c r="G25" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -5718,7 +5849,7 @@
         <v>3869.9999999999995</v>
       </c>
       <c r="G26" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="I26" s="15"/>
     </row>
@@ -5728,95 +5859,95 @@
         <v>1289999.9999999998</v>
       </c>
       <c r="G27" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F28">
         <f>F27*277.778</f>
         <v>358333619.99999994</v>
       </c>
       <c r="G28" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="I28" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F29">
         <f>F28*0.003412</f>
         <v>1222634.3114399998</v>
       </c>
       <c r="G29" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F30" s="12">
         <f>(F21*0.14)/(F29*10^6)</f>
         <v>4.1222464909102436E-6</v>
       </c>
       <c r="G30" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="I30" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F34">
         <v>21.08</v>
       </c>
       <c r="G34" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F35">
         <v>0.76</v>
       </c>
       <c r="G35" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F36" s="34">
         <f>F34*F35</f>
         <v>16.020799999999998</v>
       </c>
       <c r="G36" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -5824,7 +5955,7 @@
         <v>1.3284</v>
       </c>
       <c r="G37" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -5833,7 +5964,7 @@
         <v>21.282030719999998</v>
       </c>
       <c r="G38" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -5841,7 +5972,7 @@
         <v>1.32</v>
       </c>
       <c r="G39" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -5850,7 +5981,7 @@
         <v>28.092280550399998</v>
       </c>
       <c r="G40" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -5859,7 +5990,7 @@
         <v>4.3553923333953488</v>
       </c>
       <c r="G41" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -5867,7 +5998,7 @@
         <v>277.77800000000002</v>
       </c>
       <c r="G42" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -5876,7 +6007,7 @@
         <v>1.5679399856703368E-2</v>
       </c>
       <c r="G43" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -5884,7 +6015,7 @@
         <v>3412.14</v>
       </c>
       <c r="G44" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -5893,12 +6024,12 @@
         <v>4.5951806950193628E-6</v>
       </c>
       <c r="G45" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B47" s="18"/>
       <c r="C47" s="18"/>
@@ -5909,99 +6040,99 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F49" s="32">
         <v>6000000</v>
       </c>
       <c r="G49" s="33" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="I49" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F50">
         <v>300</v>
       </c>
       <c r="G50" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I50" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F51">
         <v>8760</v>
       </c>
       <c r="G51" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F52">
         <v>1100</v>
       </c>
       <c r="G52" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F54">
         <f>(F3*365)*F52</f>
         <v>106060240.00000001</v>
       </c>
       <c r="G54" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F55" s="34">
         <f>F54*0.003412</f>
         <v>361877.53888000007</v>
       </c>
       <c r="G55" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F56" s="12">
         <f>(F49*1.25)/(F55*10^6)</f>
         <v>2.0725243194734525E-5</v>
       </c>
       <c r="G56" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B58" s="18"/>
       <c r="C58" s="18"/>
@@ -6012,90 +6143,90 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F60">
         <f>574-184</f>
         <v>390</v>
       </c>
       <c r="G60" s="33" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F61">
         <v>3500</v>
       </c>
       <c r="G61" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I61" s="15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F62" s="32">
         <v>1500000</v>
       </c>
       <c r="G62" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I62" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F64">
         <f>F61*F62</f>
         <v>5250000000</v>
       </c>
       <c r="G64" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F65">
         <f>F64*0.003412</f>
         <v>17913000</v>
       </c>
       <c r="G65" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F66" s="25">
         <f>F60*F62</f>
         <v>585000000</v>
       </c>
       <c r="G66" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F67" s="12">
         <f>F66/(F65*10^6)</f>
         <v>3.265784625690839E-5</v>
       </c>
       <c r="G67" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -6119,108 +6250,115 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A8383B1-B2B0-41DD-8BAC-656486EFD613}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:X38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="91" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="E8" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="F8" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="G8" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="G8" s="26" t="s">
+      <c r="H8" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="I8" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="I8" s="26" t="s">
-        <v>143</v>
-      </c>
       <c r="J8" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K8" s="27"/>
       <c r="L8" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O8" s="27"/>
       <c r="P8" s="29" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="Q8" s="27"/>
       <c r="R8" s="29" t="s">
-        <v>20</v>
+        <v>386</v>
       </c>
       <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>125</v>
+      <c r="T8" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="29" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9">
         <v>0.3</v>
@@ -6228,10 +6366,10 @@
       <c r="E9">
         <v>1500</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="21">
         <v>43.754184261800326</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="21">
         <v>512727.48211595422</v>
       </c>
       <c r="H9">
@@ -6240,36 +6378,40 @@
       <c r="I9">
         <v>1000</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="21">
         <f t="shared" ref="J9:J14" si="0">AVERAGE(D9,E9)</f>
         <v>750.15</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="21">
         <f>J9*1.34102</f>
         <v>1005.9661530000001</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="21">
         <f t="shared" ref="N9:N19" si="1">F9*(((D9+E9)/2)/D9)^H9*(800/I9)</f>
         <v>191398.76147944329</v>
       </c>
       <c r="P9">
         <v>7436</v>
       </c>
-      <c r="R9">
-        <f>J9*0.003412*P9</f>
+      <c r="R9" s="43">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="T9" s="21">
+        <f t="shared" ref="T9:T19" si="2">J9*0.003412*P9</f>
         <v>19032.529744800002</v>
       </c>
-      <c r="U9" s="9">
-        <f t="shared" ref="U9:U19" si="2">N9/(R9*10^6)</f>
+      <c r="W9" s="9">
+        <f t="shared" ref="W9:W19" si="3">N9/(T9*10^6)</f>
         <v>1.005640154229821E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>126</v>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -6277,10 +6419,10 @@
       <c r="E10">
         <v>150</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="21">
         <v>1455.1962633016838</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="21">
         <v>22223.515169375642</v>
       </c>
       <c r="H10">
@@ -6289,36 +6431,40 @@
       <c r="I10">
         <v>1000</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="21">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="L10">
-        <f t="shared" ref="L10:L19" si="3">J10*1.34102</f>
+      <c r="L10" s="21">
+        <f t="shared" ref="L10:L19" si="4">J10*1.34102</f>
         <v>105.94058000000001</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="21">
         <f t="shared" si="1"/>
         <v>9793.3452423684339</v>
       </c>
       <c r="P10">
         <v>4174</v>
       </c>
-      <c r="R10">
-        <f t="shared" ref="R10:R19" si="4">J10*0.003412*P10</f>
+      <c r="R10" s="43">
+        <f>0.144/0.581</f>
+        <v>0.24784853700516352</v>
+      </c>
+      <c r="T10" s="21">
+        <f t="shared" si="2"/>
         <v>1125.0933520000001</v>
       </c>
-      <c r="U10" s="9">
-        <f t="shared" si="2"/>
+      <c r="W10" s="9">
+        <f t="shared" si="3"/>
         <v>8.7044734776536431E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>127</v>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11">
         <v>350</v>
@@ -6326,10 +6472,10 @@
       <c r="E11">
         <v>7000</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="21">
         <v>64088.852077797135</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="21">
         <v>1137028.3379406705</v>
       </c>
       <c r="H11">
@@ -6338,36 +6484,40 @@
       <c r="I11">
         <v>1000</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="21">
         <f t="shared" si="0"/>
         <v>3675</v>
       </c>
-      <c r="L11">
-        <f t="shared" si="3"/>
+      <c r="L11" s="21">
+        <f t="shared" si="4"/>
         <v>4928.2485000000006</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="21">
         <f t="shared" si="1"/>
         <v>490020.45239808032</v>
       </c>
       <c r="P11">
         <v>7436</v>
       </c>
-      <c r="R11">
-        <f t="shared" si="4"/>
+      <c r="R11" s="43">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="T11" s="21">
+        <f t="shared" si="2"/>
         <v>93240.747600000002</v>
       </c>
-      <c r="U11" s="9">
-        <f t="shared" si="2"/>
+      <c r="W11" s="9">
+        <f t="shared" si="3"/>
         <v>5.2554324692917872E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>128</v>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12">
         <v>500</v>
@@ -6375,10 +6525,10 @@
       <c r="E12">
         <v>7000</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="21">
         <v>77307.967291430425</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="21">
         <v>655523.04372978187</v>
       </c>
       <c r="H12">
@@ -6387,36 +6537,40 @@
       <c r="I12">
         <v>1000</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="21">
         <f t="shared" si="0"/>
         <v>3750</v>
       </c>
-      <c r="L12">
-        <f t="shared" si="3"/>
+      <c r="L12" s="21">
+        <f t="shared" si="4"/>
         <v>5028.8250000000007</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="21">
         <f t="shared" si="1"/>
         <v>316310.68638940249</v>
       </c>
       <c r="P12">
         <v>7436</v>
       </c>
-      <c r="R12">
-        <f t="shared" si="4"/>
+      <c r="R12" s="43">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="T12" s="21">
+        <f t="shared" si="2"/>
         <v>95143.62</v>
       </c>
-      <c r="U12" s="9">
-        <f t="shared" si="2"/>
+      <c r="W12" s="9">
+        <f t="shared" si="3"/>
         <v>3.3245601374995242E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>129</v>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D13">
         <v>0.35</v>
@@ -6424,10 +6578,10 @@
       <c r="E13">
         <v>1.8</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="21">
         <v>1297.2736980632467</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="21">
         <v>1800</v>
       </c>
       <c r="H13">
@@ -6436,36 +6590,40 @@
       <c r="I13">
         <v>1000</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="21">
         <f t="shared" si="0"/>
         <v>1.075</v>
       </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
+      <c r="L13" s="21">
+        <f t="shared" si="4"/>
         <v>1.4415964999999999</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="21">
         <f t="shared" si="1"/>
         <v>1298.941773935192</v>
       </c>
       <c r="P13">
         <v>2745</v>
       </c>
-      <c r="R13">
-        <f t="shared" si="4"/>
+      <c r="R13" s="43">
+        <f>0.048/0.581</f>
+        <v>8.2616179001721177E-2</v>
+      </c>
+      <c r="T13" s="21">
+        <f t="shared" si="2"/>
         <v>10.0683855</v>
       </c>
-      <c r="U13" s="9">
-        <f t="shared" si="2"/>
+      <c r="W13" s="9">
+        <f t="shared" si="3"/>
         <v>1.290119229081159E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>129</v>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14">
         <v>1.8</v>
@@ -6473,10 +6631,10 @@
       <c r="E14">
         <v>15</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="21">
         <v>1800</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="21">
         <v>5537.4069913635094</v>
       </c>
       <c r="H14">
@@ -6485,36 +6643,40 @@
       <c r="I14">
         <v>1000</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="21">
         <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
-      <c r="L14">
-        <f t="shared" si="3"/>
+      <c r="L14" s="21">
+        <f t="shared" si="4"/>
         <v>11.264568000000001</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="21">
         <f t="shared" si="1"/>
         <v>3257.8875198502201</v>
       </c>
       <c r="P14">
         <v>3391</v>
       </c>
-      <c r="R14">
-        <f t="shared" si="4"/>
+      <c r="R14" s="43">
+        <f>0.104/0.581</f>
+        <v>0.17900172117039587</v>
+      </c>
+      <c r="T14" s="21">
+        <f t="shared" si="2"/>
         <v>97.18877280000001</v>
       </c>
-      <c r="U14" s="9">
-        <f t="shared" si="2"/>
+      <c r="W14" s="9">
+        <f t="shared" si="3"/>
         <v>3.3521233224690123E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C15" t="s">
         <v>130</v>
-      </c>
-      <c r="C15" t="s">
-        <v>131</v>
       </c>
       <c r="D15">
         <v>0.35</v>
@@ -6522,10 +6684,10 @@
       <c r="E15">
         <v>7.5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="21">
         <v>3198.2717479261355</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="21">
         <v>22051.649944608704</v>
       </c>
       <c r="H15">
@@ -6534,36 +6696,40 @@
       <c r="I15">
         <v>1000</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="21">
         <f>AVERAGE(D15,E15)</f>
         <v>3.9249999999999998</v>
       </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
+      <c r="L15" s="21">
+        <f t="shared" si="4"/>
         <v>5.2635035000000006</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="21">
         <f t="shared" si="1"/>
         <v>11731.714005716587</v>
       </c>
       <c r="P15">
         <v>2745</v>
       </c>
-      <c r="R15">
-        <f t="shared" si="4"/>
+      <c r="R15" s="43">
+        <f>0.048/0.581</f>
+        <v>8.2616179001721177E-2</v>
+      </c>
+      <c r="T15" s="21">
+        <f t="shared" si="2"/>
         <v>36.761314500000005</v>
       </c>
-      <c r="U15" s="9">
-        <f t="shared" si="2"/>
+      <c r="W15" s="9">
+        <f t="shared" si="3"/>
         <v>3.1913205948379741E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" t="s">
         <v>132</v>
-      </c>
-      <c r="C16" t="s">
-        <v>133</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -6571,10 +6737,10 @@
       <c r="E16">
         <v>50</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="21">
         <v>1691.6842777294887</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="21">
         <v>6000</v>
       </c>
       <c r="H16">
@@ -6583,36 +6749,40 @@
       <c r="I16">
         <v>1000</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="21">
         <f t="shared" ref="J16:J19" si="5">AVERAGE(D16,E16)</f>
         <v>26.5</v>
       </c>
-      <c r="L16">
-        <f t="shared" si="3"/>
+      <c r="L16" s="21">
+        <f t="shared" si="4"/>
         <v>35.537030000000001</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="21">
         <f t="shared" si="1"/>
         <v>3607.159769818647</v>
       </c>
       <c r="P16">
         <v>3530</v>
       </c>
-      <c r="R16">
-        <f t="shared" si="4"/>
+      <c r="R16" s="43">
+        <f>0.127/0.581</f>
+        <v>0.21858864027538727</v>
+      </c>
+      <c r="T16" s="21">
+        <f t="shared" si="2"/>
         <v>319.17554000000001</v>
       </c>
-      <c r="U16" s="9">
-        <f t="shared" si="2"/>
+      <c r="W16" s="9">
+        <f t="shared" si="3"/>
         <v>1.1301491868138288E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>134</v>
+    <row r="17" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D17">
         <v>50</v>
@@ -6620,10 +6790,10 @@
       <c r="E17">
         <v>1500</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="21">
         <v>6000</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="21">
         <v>76911.661151322129</v>
       </c>
       <c r="H17">
@@ -6632,36 +6802,40 @@
       <c r="I17">
         <v>1000</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="21">
         <f t="shared" si="5"/>
         <v>775</v>
       </c>
-      <c r="L17">
-        <f t="shared" si="3"/>
+      <c r="L17" s="21">
+        <f t="shared" si="4"/>
         <v>1039.2905000000001</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="21">
         <f t="shared" si="1"/>
         <v>37496.437777254898</v>
       </c>
       <c r="P17">
         <v>7436</v>
       </c>
-      <c r="R17">
-        <f t="shared" si="4"/>
+      <c r="R17" s="43">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="T17" s="21">
+        <f t="shared" si="2"/>
         <v>19663.014800000001</v>
       </c>
-      <c r="U17" s="9">
-        <f t="shared" si="2"/>
+      <c r="W17" s="9">
+        <f t="shared" si="3"/>
         <v>1.9069526295253003E-6</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>135</v>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -6669,10 +6843,10 @@
       <c r="E18">
         <v>180</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="21">
         <v>580.86364315386913</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="21">
         <v>5300</v>
       </c>
       <c r="H18">
@@ -6681,36 +6855,40 @@
       <c r="I18">
         <v>1000</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="21">
         <f t="shared" si="5"/>
         <v>91.5</v>
       </c>
-      <c r="L18">
-        <f t="shared" si="3"/>
+      <c r="L18" s="21">
+        <f t="shared" si="4"/>
         <v>122.70333000000001</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="21">
         <f t="shared" si="1"/>
         <v>2942.2941929843073</v>
       </c>
       <c r="P18">
         <v>4174</v>
       </c>
-      <c r="R18">
-        <f t="shared" si="4"/>
+      <c r="R18" s="43">
+        <f>0.144/0.581</f>
+        <v>0.24784853700516352</v>
+      </c>
+      <c r="T18" s="21">
+        <f t="shared" si="2"/>
         <v>1303.114452</v>
       </c>
-      <c r="U18" s="9">
-        <f t="shared" si="2"/>
+      <c r="W18" s="9">
+        <f t="shared" si="3"/>
         <v>2.2578939159707113E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>135</v>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D19">
         <v>180</v>
@@ -6718,10 +6896,10 @@
       <c r="E19">
         <v>1500</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="21">
         <v>5300</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="21">
         <v>297736.10466011299</v>
       </c>
       <c r="H19">
@@ -6730,176 +6908,361 @@
       <c r="I19">
         <v>1000</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="21">
         <f t="shared" si="5"/>
         <v>840</v>
       </c>
-      <c r="L19">
-        <f t="shared" si="3"/>
+      <c r="L19" s="21">
+        <f t="shared" si="4"/>
         <v>1126.4568000000002</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="21">
         <f t="shared" si="1"/>
         <v>79155.070568115683</v>
       </c>
       <c r="P19">
         <v>7436</v>
       </c>
-      <c r="R19">
-        <f t="shared" si="4"/>
+      <c r="R19" s="43">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="T19" s="21">
+        <f t="shared" si="2"/>
         <v>21312.170880000001</v>
       </c>
-      <c r="U19" s="9">
-        <f t="shared" si="2"/>
+      <c r="W19" s="9">
+        <f t="shared" si="3"/>
         <v>3.7140782613749238E-6</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U20" s="9"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W20" s="9"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>147</v>
-      </c>
-      <c r="N21" s="21">
-        <f>AVERAGE(N9:N19)</f>
-        <v>104273.88646517909</v>
-      </c>
-      <c r="P21" s="21">
-        <f>AVERAGE(P9:P19)</f>
-        <v>5267.181818181818</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N21" s="21"/>
+      <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
-      <c r="R21" s="21">
-        <f>AVERAGE(R9:R19)</f>
+      <c r="T21" s="21">
+        <f>AVERAGE(T9:T19)</f>
         <v>22843.953167418182</v>
       </c>
-      <c r="U21" s="9">
-        <f>AVERAGE(U9:U19)</f>
+      <c r="W21" s="9">
+        <f>AVERAGE(W9:W19)</f>
         <v>4.8016954538032345E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>156</v>
-      </c>
-      <c r="N22" s="21">
-        <f>((N13+N15)/2)*(58.8/96.2)+(N14)*(26.4/96.2)+(N16)*(9.1/96.2)+((N10+N18)/2)*(1.8/96.2)+((N9+N11+N12+N17+N19)/5)*(0.1/96.2)</f>
-        <v>5568.4445739627981</v>
-      </c>
-      <c r="P22" s="21">
-        <f>((P13+P15)/2)*(58.8/96.2)+(P14)*(26.4/96.2)+(P16)*(9.1/96.2)+((P10+P18)/2)*(1.8/96.2)+((P9+P11+P12+P17+P19)/5)*(0.1/96.2)</f>
-        <v>3028.1517671517663</v>
-      </c>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="N22" s="21"/>
+      <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
-      <c r="R22" s="21">
-        <f>((R13+R15)/2)*(58.8/96.2)+(R14)*(26.4/96.2)+(R16)*(9.1/96.2)+((R10+R18)/2)*(1.8/96.2)+((R9+R11+R12+R17+R19)/5)*(0.1/96.2)</f>
-        <v>145.53329397106029</v>
-      </c>
-      <c r="U22" s="12">
-        <f>((U13+U15)/2)*(58.8/96.2)+(U14)*(26.4/96.2)+(U16)*(9.1/96.2)+((U10+U18)/2)*(1.8/96.2)+((U9+U11+U12+U17+U19)/5)*(0.1/96.2)</f>
-        <v>1.4733459973606227E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="U23" s="9"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="T22" s="47">
+        <f>SUMPRODUCT(F24:F28, I24:I28)</f>
+        <v>13814.301562165096</v>
+      </c>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="48">
+        <f>SUMPRODUCT(F24:F28, N24:N28)</f>
+        <v>2.9652197760109964E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C23" s="49" t="s">
+        <v>388</v>
+      </c>
+      <c r="D23" s="49"/>
+      <c r="E23" s="49"/>
+      <c r="F23" s="49" t="s">
+        <v>397</v>
+      </c>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49" t="s">
+        <v>398</v>
+      </c>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50" t="s">
+        <v>394</v>
+      </c>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="T23" s="21"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C24" s="52" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="55">
+        <f>0.048/0.581</f>
+        <v>8.2616179001721177E-2</v>
+      </c>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="58">
+        <f>((T13+T15)/2)</f>
+        <v>23.414850000000001</v>
+      </c>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="51">
+        <f>((W13+W15)/2)</f>
+        <v>2.2407199119595664E-4</v>
+      </c>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="T24" s="21"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C25" s="52" t="s">
+        <v>392</v>
+      </c>
+      <c r="D25" s="53"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="55">
+        <f>0.104/0.581</f>
+        <v>0.17900172117039587</v>
+      </c>
+      <c r="G25" s="56"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="58">
+        <f>T14</f>
+        <v>97.18877280000001</v>
+      </c>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="51">
+        <f>W14</f>
+        <v>3.3521233224690123E-5</v>
+      </c>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="T25" s="21"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C26" s="52" t="s">
+        <v>390</v>
+      </c>
+      <c r="D26" s="53"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="55">
+        <f>0.127/0.581</f>
+        <v>0.21858864027538727</v>
+      </c>
+      <c r="G26" s="56"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="58">
+        <f>T16</f>
+        <v>319.17554000000001</v>
+      </c>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="51">
+        <f>W16</f>
+        <v>1.1301491868138288E-5</v>
+      </c>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="T26" s="21"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C27" s="52" t="s">
+        <v>389</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="55">
+        <f>0.144/0.581</f>
+        <v>0.24784853700516352</v>
+      </c>
+      <c r="G27" s="56"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="58">
+        <f>((T10+T18)/2)</f>
+        <v>1214.1039020000001</v>
+      </c>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="51">
+        <f>((W10+W18)/2)</f>
+        <v>5.481183696812177E-6</v>
+      </c>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="T27" s="21"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C28" s="52" t="s">
+        <v>393</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="55">
+        <f>0.157/0.581</f>
+        <v>0.27022375215146299</v>
+      </c>
+      <c r="G28" s="56"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="58">
+        <f>((T9+T11+T12+T17+T19)/5)</f>
+        <v>49678.416604960003</v>
+      </c>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="51">
+        <f>((W9+W11+W12+W17+W19)/5)</f>
+        <v>4.8514850079979492E-6</v>
+      </c>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="T28" s="21"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U29" s="9"/>
+      <c r="W29" s="9"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="U32" s="9"/>
+      <c r="W32" s="9"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>286</v>
+      </c>
+      <c r="D33" s="21">
+        <v>502</v>
+      </c>
+      <c r="E33" t="s">
+        <v>164</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="T33" s="9"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="21">
+        <v>250</v>
+      </c>
+      <c r="E34" t="s">
         <v>289</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="G26" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="G34" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="D27" s="34">
-        <v>502</v>
-      </c>
-      <c r="E27" t="s">
-        <v>168</v>
-      </c>
-      <c r="G27" s="15" t="s">
+      <c r="T34" s="9"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="D35" s="21">
+        <f>D34/1.341</f>
+        <v>186.42803877703207</v>
+      </c>
+      <c r="E35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>292</v>
       </c>
-      <c r="D28" s="34">
-        <v>250</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D36" s="21">
+        <v>2080</v>
+      </c>
+      <c r="E36" t="s">
+        <v>216</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="21">
+        <f>D35*0.003412*D36</f>
+        <v>1323.0723340790455</v>
+      </c>
+      <c r="E37" t="s">
         <v>293</v>
       </c>
-      <c r="G28" s="15" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>295</v>
-      </c>
-      <c r="D29" s="34">
-        <f>D28/1.341</f>
-        <v>186.42803877703207</v>
-      </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>296</v>
-      </c>
-      <c r="D30" s="34">
-        <v>2080</v>
-      </c>
-      <c r="E30" t="s">
-        <v>220</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="I30" s="8"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="34">
-        <f>D29*0.003412*D30</f>
-        <v>1323.0723340790455</v>
-      </c>
-      <c r="E31" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="41">
-        <f>(D27*D29)/(D31*10^6)</f>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>145</v>
+      </c>
+      <c r="D38" s="12">
+        <f>(D33*D35)/(D37*10^6)</f>
         <v>7.0734511678239686E-5</v>
       </c>
-      <c r="E32" t="s">
-        <v>146</v>
+      <c r="E38" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="I25:M25"/>
+    <mergeCell ref="I26:M26"/>
+    <mergeCell ref="I27:M27"/>
+    <mergeCell ref="I28:M28"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G27" r:id="rId1" xr:uid="{89D540DE-65F8-419E-8E02-FD08F0D4350B}"/>
-    <hyperlink ref="G28" r:id="rId2" xr:uid="{2BEBA02A-CA41-4A57-93D0-D9F4D2610A4F}"/>
-    <hyperlink ref="G30" r:id="rId3" xr:uid="{098A2275-9E62-4836-8A3D-FE6E71782B1D}"/>
+    <hyperlink ref="G33" r:id="rId1" xr:uid="{89D540DE-65F8-419E-8E02-FD08F0D4350B}"/>
+    <hyperlink ref="G34" r:id="rId2" xr:uid="{2BEBA02A-CA41-4A57-93D0-D9F4D2610A4F}"/>
+    <hyperlink ref="G36" r:id="rId3" xr:uid="{098A2275-9E62-4836-8A3D-FE6E71782B1D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId4"/>
@@ -6920,7 +7283,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -6931,12 +7294,12 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6944,94 +7307,94 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D6">
         <f>AVERAGE(760,1000)</f>
         <v>880</v>
       </c>
       <c r="E6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D7">
         <f>AVERAGE(373.1,597)</f>
         <v>485.05</v>
       </c>
       <c r="E7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D11">
         <f>AVERAGE(975,1200)</f>
         <v>1087.5</v>
       </c>
       <c r="E11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D12">
         <f>AVERAGE(1492.5,2238.8)</f>
         <v>1865.65</v>
       </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D15">
         <v>1.5</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D16">
         <v>70</v>
       </c>
       <c r="E16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G18">
         <f>(D6)*(1.5*1000000)</f>
@@ -7040,7 +7403,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G19">
         <f>(1.5*1000000)*(0.7*8760)</f>
@@ -7049,7 +7412,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G20">
         <f>G19*3412</f>
@@ -7058,7 +7421,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G21">
         <f>G18/G20</f>
@@ -7067,7 +7430,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G22">
         <f>(D7*(1.5*1000000))/G20</f>
@@ -7076,7 +7439,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G24">
         <f>(D11)*(1.5*1000000)</f>
@@ -7085,7 +7448,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G25">
         <f>(1.5*1000000)*(0.7*8760)</f>
@@ -7094,7 +7457,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G26">
         <f>G25*3412</f>
@@ -7103,7 +7466,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G27">
         <f>G24/G26</f>
@@ -7112,7 +7475,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G28">
         <f>(D12*(1.5*1000000))/G26</f>
@@ -7121,12 +7484,12 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G32" s="12">
         <f>(G21*0.75)+(G27*0.25)</f>
@@ -7135,7 +7498,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G33" s="9">
         <f>G32*0.6</f>
@@ -7147,7 +7510,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G35" s="9">
         <f>(G22*0.75)+(G28*0.25)</f>
@@ -7175,7 +7538,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -7187,184 +7550,184 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E3" s="39">
         <f>2758*1.03</f>
         <v>2840.7400000000002</v>
       </c>
       <c r="F3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E4">
         <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <f>18*365</f>
         <v>6570</v>
       </c>
       <c r="F5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="H5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E7">
         <f>E4*E5</f>
         <v>118260</v>
       </c>
       <c r="F7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E8">
         <f>E7*0.003412</f>
         <v>403.50312000000002</v>
       </c>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E9" s="12">
         <f>E3/(E8*10^6)</f>
         <v>7.0401933942914745E-6</v>
       </c>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B16" s="8">
         <v>862500</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B17" s="8">
         <v>1500000</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B18" s="8">
         <f>AVERAGE(B16,B17)</f>
         <v>1181250</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="32">
         <v>8760</v>
       </c>
       <c r="C20" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B21" s="32">
         <v>6051100</v>
       </c>
       <c r="C21" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B23">
         <f>B20*B21</f>
         <v>53007636000</v>
       </c>
       <c r="C23" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B24" s="12">
         <f>B18/B23</f>
         <v>2.2284525195577483E-5</v>
       </c>
       <c r="C24" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -7380,7 +7743,7 @@
   <sheetPr>
     <tabColor theme="3" tint="0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7392,42 +7755,42 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="12">
         <f>Boilers!$A$18</f>
@@ -7471,7 +7834,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="10">
         <f>B2</f>
@@ -7516,7 +7879,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="12">
         <f>'NB Medium Temp'!D40</f>
@@ -7560,7 +7923,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="12">
         <f>'NB High Temp'!F10</f>
@@ -7604,7 +7967,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="12">
         <f>Cooling!$B$49</f>
@@ -7648,11 +8011,11 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="12">
-        <f>'Machine Drive'!$U$22</f>
-        <v>1.4733459973606227E-4</v>
+        <f>'Machine Drive'!$W$22</f>
+        <v>2.9652197760109964E-5</v>
       </c>
       <c r="C7" s="10">
         <f>$F$7</f>
@@ -7667,7 +8030,7 @@
         <v>7.0734511678239686E-5</v>
       </c>
       <c r="F7" s="12">
-        <f>'Machine Drive'!D32</f>
+        <f>'Machine Drive'!D38</f>
         <v>7.0734511678239686E-5</v>
       </c>
       <c r="G7" s="40">
@@ -7692,7 +8055,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="12">
         <f>Electrochemical!$G32</f>
@@ -7728,7 +8091,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="12">
         <f>Other!E9</f>
@@ -7772,37 +8135,32 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>388</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>